<commit_message>
add test base and contact manager test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestFramework.xlsx
+++ b/src/test/resources/TestFramework.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>http://localhost:8880/ab/ContactManager.do</t>
+  </si>
+  <si>
+    <t>TS007</t>
+  </si>
+  <si>
+    <t>TS008</t>
+  </si>
+  <si>
+    <t>SETTING</t>
+  </si>
+  <si>
+    <t>Stevens</t>
+  </si>
+  <si>
+    <t>COMPANYNAME</t>
   </si>
 </sst>
 </file>
@@ -149,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -206,6 +233,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,10 +560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,8 +571,8 @@
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -767,11 +796,148 @@
         <v>10</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E15" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test add new contact
</commit_message>
<xml_diff>
--- a/src/test/resources/TestFramework.xlsx
+++ b/src/test/resources/TestFramework.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="39">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>COMPANYNAME</t>
+  </si>
+  <si>
+    <t>ADD_NEW_CONTACT</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -235,6 +238,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,14 +527,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -537,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -545,7 +550,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -560,22 +565,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -592,7 +597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -609,7 +614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -626,7 +631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -643,7 +648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -660,7 +665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -677,7 +682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -694,7 +699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
@@ -711,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -728,7 +733,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -745,7 +750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -762,7 +767,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -779,7 +784,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
@@ -796,7 +801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>31</v>
       </c>
@@ -813,7 +818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
@@ -830,7 +835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
@@ -847,7 +852,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>31</v>
       </c>
@@ -864,7 +869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>31</v>
       </c>
@@ -881,7 +886,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>31</v>
       </c>
@@ -898,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>31</v>
       </c>
@@ -915,7 +920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>31</v>
       </c>
@@ -930,14 +935,83 @@
       </c>
       <c r="E21" s="8" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E15" r:id="rId2"/>
+    <hyperlink ref="E23" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>